<commit_message>
Your descriptive message about the changes
</commit_message>
<xml_diff>
--- a/livedata.xlsx
+++ b/livedata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sajid.DESKTOP-5LISAEP\OneDrive\Desktop\a2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sajid.DESKTOP-5LISAEP\OneDrive\Desktop\a2\githubdata\sajid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64240DA6-1D36-41F4-90E4-00FE3A601989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C7F78C-01DB-4619-A7A1-3BE262F3E431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{058D3E5C-831A-4C5B-A8D7-136C208A779A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>ff</t>
+  </si>
+  <si>
+    <t>kk</t>
   </si>
 </sst>
 </file>
@@ -430,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6975CA7F-12A3-44B7-AC7D-31DDDEECA4BE}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -494,6 +497,14 @@
         <v>100</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated files with modifications
</commit_message>
<xml_diff>
--- a/livedata.xlsx
+++ b/livedata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sajid.DESKTOP-5LISAEP\OneDrive\Desktop\gm\sajid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sajid.DESKTOP-5LISAEP\OneDrive\Desktop\aaa\sajid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA88453B-AFC9-4359-8A70-33BA223335E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D0522E-4A5B-4941-A6DD-C6851E93FF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1245" windowWidth="8745" windowHeight="9780" xr2:uid="{058D3E5C-831A-4C5B-A8D7-136C208A779A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{058D3E5C-831A-4C5B-A8D7-136C208A779A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6975CA7F-12A3-44B7-AC7D-31DDDEECA4BE}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -560,6 +560,14 @@
         <v>334</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>